<commit_message>
Revert "Merge branch 'xuhan'"
This reverts commit e0a11b99069e156ad44c14aa05f09dcd358c9b61.
</commit_message>
<xml_diff>
--- a/作业完成情况汇总.xlsx
+++ b/作业完成情况汇总.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70">
   <si>
     <t>WHJ171103班晚自习作业完成情况汇总表</t>
   </si>
@@ -88,6 +88,9 @@
     <t>几乎没有进度</t>
   </si>
   <si>
+    <t>有进步</t>
+  </si>
+  <si>
     <t>刘鹏</t>
   </si>
   <si>
@@ -125,6 +128,9 @@
   </si>
   <si>
     <t>董加丰</t>
+  </si>
+  <si>
+    <t>游戏还有一点</t>
   </si>
   <si>
     <t>李晓楠</t>
@@ -204,6 +210,9 @@
   </si>
   <si>
     <t>数据存到xml初步完成</t>
+  </si>
+  <si>
+    <t>提交有异常</t>
   </si>
   <si>
     <t>沈世伟</t>
@@ -225,8 +234,8 @@
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -259,46 +268,25 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -309,8 +297,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -324,9 +342,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -341,14 +366,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -373,17 +398,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -393,14 +410,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -423,127 +432,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,42 +613,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,6 +667,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -683,21 +731,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -714,24 +747,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -744,17 +764,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -763,10 +772,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -775,137 +784,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -943,9 +952,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1268,17 +1274,17 @@
   <sheetPr/>
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="6" width="9.63333333333333" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.13333333333333" style="1"/>
-    <col min="8" max="8" width="49.1666666666667" style="1" customWidth="1"/>
-    <col min="9" max="10" width="9" style="1"/>
+    <col min="7" max="8" width="9.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.13333333333333" style="1"/>
+    <col min="10" max="10" width="49.1666666666667" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1348,12 +1354,14 @@
         <v>43083</v>
       </c>
       <c r="H4" s="6"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
+      <c r="I4" s="5">
+        <v>43084</v>
+      </c>
+      <c r="J4" s="6"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
     </row>
     <row r="5" ht="25" customHeight="1" spans="1:14">
       <c r="A5" s="3" t="s">
@@ -1380,12 +1388,16 @@
       <c r="H5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
+      <c r="I5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
     </row>
     <row r="6" ht="25" customHeight="1" spans="1:14">
       <c r="A6" s="3" t="s">
@@ -1406,12 +1418,14 @@
         <v>8</v>
       </c>
       <c r="H6" s="4"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
+      <c r="I6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:14">
       <c r="A7" s="3" t="s">
@@ -1432,12 +1446,14 @@
         <v>8</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
+      <c r="I7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
     </row>
     <row r="8" ht="25" customHeight="1" spans="1:14">
       <c r="A8" s="3" t="s">
@@ -1460,12 +1476,14 @@
         <v>8</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
+      <c r="I8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
     </row>
     <row r="9" ht="25" customHeight="1" spans="1:14">
       <c r="A9" s="7" t="s">
@@ -1482,14 +1500,16 @@
         <v>8</v>
       </c>
       <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
+      <c r="G9" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="H9" s="10"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
     </row>
     <row r="10" ht="25" customHeight="1" spans="1:14">
       <c r="A10" s="3" t="s">
@@ -1510,12 +1530,12 @@
         <v>8</v>
       </c>
       <c r="H10" s="4"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
     </row>
     <row r="11" ht="25" customHeight="1" spans="1:14">
       <c r="A11" s="3"/>
@@ -1530,14 +1550,16 @@
         <v>12</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="G11" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="H11" s="4"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
     </row>
     <row r="12" ht="25" customHeight="1" spans="1:14">
       <c r="A12" s="3"/>
@@ -1558,12 +1580,14 @@
       <c r="H12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
+      <c r="I12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
     </row>
     <row r="13" ht="25" customHeight="1" spans="1:14">
       <c r="A13" s="3"/>
@@ -1580,21 +1604,25 @@
         <v>8</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
+      <c r="G13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
     </row>
     <row r="14" ht="25" customHeight="1" spans="1:14">
       <c r="A14" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>8</v>
@@ -1604,21 +1632,25 @@
         <v>8</v>
       </c>
       <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="G14" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="H14" s="9"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
+      <c r="I14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="9"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
     </row>
     <row r="15" ht="25" customHeight="1" spans="1:14">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>8</v>
@@ -1630,23 +1662,23 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
     </row>
     <row r="16" ht="25" customHeight="1" spans="1:14">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>12</v>
@@ -1656,17 +1688,19 @@
         <v>8</v>
       </c>
       <c r="H16" s="4"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
+      <c r="I16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
     </row>
     <row r="17" ht="25" customHeight="1" spans="1:14">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>20</v>
@@ -1678,17 +1712,17 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
     </row>
     <row r="18" ht="25" customHeight="1" spans="1:14">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>8</v>
@@ -1698,21 +1732,25 @@
         <v>8</v>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="G18" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="H18" s="4"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
+      <c r="I18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="4"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
     </row>
     <row r="19" ht="25" customHeight="1" spans="1:14">
       <c r="A19" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>8</v>
@@ -1722,21 +1760,25 @@
         <v>8</v>
       </c>
       <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+      <c r="G19" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="H19" s="9"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
+      <c r="I19" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" s="9"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
     </row>
     <row r="20" ht="25" customHeight="1" spans="1:14">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>8</v>
@@ -1748,23 +1790,23 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
     </row>
     <row r="21" ht="25" customHeight="1" spans="1:14">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>8</v>
@@ -1772,20 +1814,20 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
     </row>
     <row r="22" ht="25" customHeight="1" spans="1:14">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="12" t="s">
@@ -1794,17 +1836,17 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
     </row>
     <row r="23" ht="25" customHeight="1" spans="1:14">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>8</v>
@@ -1814,21 +1856,27 @@
         <v>8</v>
       </c>
       <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
+      <c r="G23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J23" s="4"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
     </row>
     <row r="24" ht="25" customHeight="1" spans="1:14">
       <c r="A24" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>8</v>
@@ -1838,21 +1886,25 @@
         <v>8</v>
       </c>
       <c r="F24" s="9"/>
-      <c r="G24" s="11"/>
+      <c r="G24" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="H24" s="9"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
+      <c r="I24" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J24" s="9"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
     </row>
     <row r="25" ht="25" customHeight="1" spans="1:14">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>8</v>
@@ -1864,23 +1916,23 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
     </row>
     <row r="26" ht="25" customHeight="1" spans="1:14">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>8</v>
@@ -1888,17 +1940,17 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
     </row>
     <row r="27" ht="25" customHeight="1" spans="1:14">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>8</v>
@@ -1910,20 +1962,20 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
     </row>
     <row r="28" ht="25" customHeight="1" spans="1:14">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="12" t="s">
@@ -1932,19 +1984,19 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
     </row>
     <row r="29" ht="25" customHeight="1" spans="1:14">
       <c r="A29" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>8</v>
@@ -1956,25 +2008,25 @@
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
     </row>
     <row r="30" ht="25" customHeight="1" spans="1:14">
       <c r="A30" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>8</v>
@@ -1984,25 +2036,25 @@
         <v>8</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
+        <v>49</v>
+      </c>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
     </row>
     <row r="31" ht="25" customHeight="1" spans="1:14">
       <c r="A31" s="3"/>
       <c r="B31" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>8</v>
@@ -2011,23 +2063,23 @@
         <v>8</v>
       </c>
       <c r="H31" s="4"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
     </row>
     <row r="32" ht="25" customHeight="1" spans="1:14">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>8</v>
@@ -2035,23 +2087,23 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
     </row>
     <row r="33" ht="25" customHeight="1" spans="1:14">
       <c r="A33" s="3"/>
       <c r="B33" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>12</v>
@@ -2061,27 +2113,29 @@
         <v>12</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
+        <v>56</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J33" s="4"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
     </row>
     <row r="34" ht="25" customHeight="1" spans="1:14">
       <c r="A34" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>8</v>
@@ -2091,27 +2145,29 @@
         <v>8</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
+        <v>60</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J34" s="9"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
     </row>
     <row r="35" ht="25" customHeight="1" spans="1:14">
       <c r="A35" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E35" s="12" t="s">
         <v>12</v>
@@ -2121,47 +2177,51 @@
         <v>8</v>
       </c>
       <c r="H35" s="4"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
+      <c r="I35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J35" s="4"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
     </row>
     <row r="36" ht="25" customHeight="1" spans="1:14">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E36" s="12" t="s">
         <v>8</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
+      <c r="H36" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
     </row>
     <row r="37" ht="25" customHeight="1" spans="1:14">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E37" s="12" t="s">
         <v>12</v>
@@ -2169,23 +2229,25 @@
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
+      <c r="I37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J37" s="4"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
     </row>
     <row r="38" ht="25" customHeight="1" spans="1:14">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E38" s="12" t="s">
         <v>8</v>
@@ -2193,19 +2255,20 @@
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A20:A23"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "我"""
This reverts commit 8e03048b821c37539979dca97cd8a5f2cfaf4949.
</commit_message>
<xml_diff>
--- a/作业完成情况汇总.xlsx
+++ b/作业完成情况汇总.xlsx
@@ -223,10 +223,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -253,6 +253,29 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -319,8 +342,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -355,46 +395,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
@@ -423,6 +423,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -471,6 +501,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -513,12 +561,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -538,48 +580,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,6 +658,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -675,9 +714,20 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -705,56 +755,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -763,145 +763,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1266,7 +1266,7 @@
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1783,9 +1783,7 @@
         <v>8</v>
       </c>
       <c r="J19" s="9"/>
-      <c r="K19" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="K19" s="9"/>
       <c r="L19" s="9"/>
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
@@ -1891,9 +1889,7 @@
         <v>8</v>
       </c>
       <c r="J23" s="9"/>
-      <c r="K23" s="11" t="s">
-        <v>8</v>
-      </c>
+      <c r="K23" s="11"/>
       <c r="L23" s="9"/>
       <c r="M23" s="13"/>
       <c r="N23" s="13"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Revert "我""""
This reverts commit cf9f03e2384c96d82f35092ef09b19e1f1124108.
</commit_message>
<xml_diff>
--- a/作业完成情况汇总.xlsx
+++ b/作业完成情况汇总.xlsx
@@ -223,10 +223,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -253,29 +253,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -342,25 +319,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -395,6 +355,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
@@ -423,6 +423,144 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -441,145 +579,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,45 +658,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -714,20 +675,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -755,6 +705,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -763,10 +763,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -775,133 +775,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1266,7 +1266,7 @@
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1783,7 +1783,9 @@
         <v>8</v>
       </c>
       <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
+      <c r="K19" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="L19" s="9"/>
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
@@ -1889,7 +1891,9 @@
         <v>8</v>
       </c>
       <c r="J23" s="9"/>
-      <c r="K23" s="11"/>
+      <c r="K23" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="L23" s="9"/>
       <c r="M23" s="13"/>
       <c r="N23" s="13"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' into xx"
This reverts commit 88fcacc2cfc15c7c711ec9cc11db7a69c8ab8873.
</commit_message>
<xml_diff>
--- a/作业完成情况汇总.xlsx
+++ b/作业完成情况汇总.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="12645"/>
+    <workbookView windowWidth="28695" windowHeight="13065"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -223,9 +223,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -260,6 +260,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -326,24 +333,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -364,10 +370,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -386,21 +401,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -423,6 +423,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -471,6 +495,78 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -489,84 +585,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -580,30 +604,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -682,6 +682,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -712,30 +736,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -763,145 +763,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1266,7 +1266,7 @@
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1705,9 +1705,7 @@
         <v>8</v>
       </c>
       <c r="J16" s="4"/>
-      <c r="K16" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "11"""
This reverts commit a3005a05f7b8e7268be185dce6fd892e78951589.
</commit_message>
<xml_diff>
--- a/作业完成情况汇总.xlsx
+++ b/作业完成情况汇总.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050"/>
+    <workbookView windowWidth="28695" windowHeight="13665"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -223,10 +223,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -259,67 +259,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -342,9 +281,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -358,6 +312,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -366,15 +334,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -387,16 +363,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -423,187 +423,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,30 +658,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -697,28 +673,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -747,11 +715,43 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -763,10 +763,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -775,133 +775,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1001,11 +1001,6 @@
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1261,16 +1256,17 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1925,9 +1921,7 @@
         <v>8</v>
       </c>
       <c r="J24" s="4"/>
-      <c r="K24" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="13"/>
       <c r="N24" s="13"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Revert "11""""
This reverts commit fa912069c72d0f16b7fc691fb45de6c042a80767.
</commit_message>
<xml_diff>
--- a/作业完成情况汇总.xlsx
+++ b/作业完成情况汇总.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13665"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -223,10 +223,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -259,6 +259,67 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -281,24 +342,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -312,20 +358,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -334,23 +366,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -363,40 +387,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -423,13 +423,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -441,169 +579,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,6 +658,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -673,20 +697,28 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -715,43 +747,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -763,145 +763,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1001,6 +1001,11 @@
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1256,17 +1261,16 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1921,7 +1925,9 @@
         <v>8</v>
       </c>
       <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
+      <c r="K24" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="L24" s="4"/>
       <c r="M24" s="13"/>
       <c r="N24" s="13"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Revert "Revert "11"""""
This reverts commit 74624ea2922d76cd4a485944dc8edc7aaee273dc.
</commit_message>
<xml_diff>
--- a/作业完成情况汇总.xlsx
+++ b/作业完成情况汇总.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050"/>
+    <workbookView windowWidth="28695" windowHeight="13665"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -223,10 +223,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -259,67 +259,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -342,9 +281,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -358,6 +312,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -366,15 +334,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -387,16 +363,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -423,187 +423,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,30 +658,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -697,28 +673,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -747,11 +715,43 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -763,10 +763,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -775,133 +775,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1001,11 +1001,6 @@
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1261,16 +1256,17 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1925,9 +1921,7 @@
         <v>8</v>
       </c>
       <c r="J24" s="4"/>
-      <c r="K24" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="13"/>
       <c r="N24" s="13"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Revert "Revert "Revert "11""""""
This reverts commit 8ddefadc2979016dcedd504c67a8f8c634ca52c1.
</commit_message>
<xml_diff>
--- a/作业完成情况汇总.xlsx
+++ b/作业完成情况汇总.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13665"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -223,10 +223,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -259,6 +259,67 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -281,24 +342,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -312,20 +358,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -334,23 +366,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -363,40 +387,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -423,13 +423,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -441,169 +579,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,6 +658,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -673,20 +697,28 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -715,43 +747,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -763,145 +763,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1001,6 +1001,11 @@
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1256,17 +1261,16 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1921,7 +1925,9 @@
         <v>8</v>
       </c>
       <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
+      <c r="K24" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="L24" s="4"/>
       <c r="M24" s="13"/>
       <c r="N24" s="13"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Revert "Revert "Revert "Revert "11"""""""
This reverts commit 4897513e175e45a642e787f8c2cfc0cf26133c91.
</commit_message>
<xml_diff>
--- a/作业完成情况汇总.xlsx
+++ b/作业完成情况汇总.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050"/>
+    <workbookView windowWidth="28695" windowHeight="13665"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -223,10 +223,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -259,67 +259,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -342,9 +281,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -358,6 +312,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -366,15 +334,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -387,16 +363,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -423,187 +423,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,30 +658,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -697,28 +673,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -747,11 +715,43 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -763,10 +763,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -775,133 +775,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1001,11 +1001,6 @@
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1261,16 +1256,17 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1925,9 +1921,7 @@
         <v>8</v>
       </c>
       <c r="J24" s="4"/>
-      <c r="K24" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="13"/>
       <c r="N24" s="13"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Revert "Revert "Revert "Revert "Revert "11""""""""
This reverts commit a9c2f1a42865b9ade8dab21fba666cd0f3035fad.
</commit_message>
<xml_diff>
--- a/作业完成情况汇总.xlsx
+++ b/作业完成情况汇总.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13665"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -223,10 +223,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -259,6 +259,67 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -281,24 +342,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -312,20 +358,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -334,23 +366,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -363,40 +387,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -423,13 +423,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -441,169 +579,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,6 +658,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -673,20 +697,28 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -715,43 +747,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -763,145 +763,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1001,6 +1001,11 @@
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1256,17 +1261,16 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1921,7 +1925,9 @@
         <v>8</v>
       </c>
       <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
+      <c r="K24" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="L24" s="4"/>
       <c r="M24" s="13"/>
       <c r="N24" s="13"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "1"""
This reverts commit 295dc87116a38b99a073ed6574a1cadd02a9f642.
</commit_message>
<xml_diff>
--- a/作业完成情况汇总.xlsx
+++ b/作业完成情况汇总.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69">
   <si>
     <t>WHJ171103班晚自习作业完成情况汇总表</t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>没有理清解题思路</t>
-  </si>
-  <si>
-    <t>只完成了作业2和增</t>
   </si>
   <si>
     <t>董加丰</t>
@@ -232,10 +229,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -269,65 +266,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -343,6 +282,30 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -372,6 +335,41 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -396,16 +394,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -432,13 +429,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,115 +459,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -576,43 +609,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -667,6 +664,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -682,17 +703,37 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -715,50 +756,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -772,10 +769,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -784,19 +781,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -805,112 +802,112 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1276,7 +1273,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1935,17 +1932,13 @@
         <v>8</v>
       </c>
       <c r="N20" s="4"/>
-      <c r="O20" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="P20" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
     </row>
     <row r="21" ht="25" customHeight="1" spans="1:16">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>8</v>
@@ -1959,7 +1952,7 @@
         <v>12</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>8</v>
@@ -1977,7 +1970,7 @@
         <v>12</v>
       </c>
       <c r="P21" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" ht="25" customHeight="1" spans="1:16">
@@ -1985,7 +1978,7 @@
         <v>14</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>8</v>
@@ -2015,7 +2008,7 @@
         <v>12</v>
       </c>
       <c r="P22" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" ht="25" customHeight="1" spans="1:16">
@@ -2023,7 +2016,7 @@
         <v>16</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>8</v>
@@ -2053,13 +2046,13 @@
     <row r="24" ht="25" customHeight="1" spans="1:16">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>8</v>
@@ -2085,13 +2078,13 @@
         <v>12</v>
       </c>
       <c r="P24" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" ht="25" customHeight="1" spans="1:16">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>8</v>
@@ -2127,7 +2120,7 @@
         <v>14</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>8</v>
@@ -2163,13 +2156,13 @@
         <v>16</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>8</v>
@@ -2179,7 +2172,7 @@
         <v>8</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>8</v>
@@ -2201,13 +2194,13 @@
     <row r="28" ht="25" customHeight="1" spans="1:16">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>8</v>
@@ -2234,13 +2227,13 @@
     <row r="29" ht="25" customHeight="1" spans="1:16">
       <c r="A29" s="3"/>
       <c r="B29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>12</v>
@@ -2250,7 +2243,7 @@
         <v>12</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>8</v>
@@ -2268,7 +2261,7 @@
         <v>12</v>
       </c>
       <c r="P29" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" ht="25" customHeight="1" spans="1:16">
@@ -2276,13 +2269,13 @@
         <v>14</v>
       </c>
       <c r="B30" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="D30" s="11" t="s">
         <v>56</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>57</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>8</v>
@@ -2292,7 +2285,7 @@
         <v>8</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I30" s="9" t="s">
         <v>8</v>
@@ -2314,13 +2307,13 @@
         <v>16</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>12</v>
@@ -2346,19 +2339,19 @@
         <v>12</v>
       </c>
       <c r="P31" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" ht="25" customHeight="1" spans="1:16">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>8</v>
@@ -2366,7 +2359,7 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>8</v>
@@ -2384,19 +2377,19 @@
         <v>12</v>
       </c>
       <c r="P32" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" ht="25" customHeight="1" spans="1:16">
       <c r="A33" s="3"/>
       <c r="B33" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>12</v>
@@ -2422,13 +2415,13 @@
     <row r="34" ht="25" customHeight="1" spans="1:16">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="E34" s="12" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Revert "Revert "Revert "fw"""
This reverts commit a5ba74214244436fa891c16b2f8b7edbc39bda05, reversing
changes made to 801a711594812293d6a6e974023f273c0c08f4b3.
</commit_message>
<xml_diff>
--- a/作业完成情况汇总.xlsx
+++ b/作业完成情况汇总.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24180" windowHeight="13065"/>
+    <workbookView windowWidth="28695" windowHeight="13065"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44">
   <si>
     <t>WHJ171103班晚自习作业完成情况汇总表</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>冯文</t>
+  </si>
+  <si>
+    <t>修改有问题</t>
   </si>
   <si>
     <t>沈世伟</t>
@@ -150,10 +153,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -192,6 +195,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -200,6 +211,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
@@ -215,6 +234,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -222,24 +256,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -260,14 +318,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -275,59 +325,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -398,6 +401,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -440,18 +491,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -495,42 +534,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -600,26 +603,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -641,9 +644,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -658,27 +663,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -690,10 +693,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -705,130 +708,130 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1189,8 +1192,8 @@
   <sheetPr/>
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1854,10 +1857,10 @@
       <c r="C32" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="12" t="s">
-        <v>8</v>
-      </c>
+      <c r="D32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="12"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -1871,7 +1874,7 @@
     <row r="33" ht="24.95" customHeight="1" spans="1:14">
       <c r="A33" s="3"/>
       <c r="B33" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>8</v>
@@ -1891,13 +1894,13 @@
     <row r="34" ht="42" customHeight="1" spans="1:14">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="4"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Revert "fw""""
This reverts commit 1d7b73a8a04a3d28321449087bf7b8e52e59ea3b.
</commit_message>
<xml_diff>
--- a/作业完成情况汇总.xlsx
+++ b/作业完成情况汇总.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13065"/>
+    <workbookView windowWidth="24180" windowHeight="13065"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43">
   <si>
     <t>WHJ171103班晚自习作业完成情况汇总表</t>
   </si>
@@ -134,9 +134,6 @@
   </si>
   <si>
     <t>冯文</t>
-  </si>
-  <si>
-    <t>修改有问题</t>
   </si>
   <si>
     <t>沈世伟</t>
@@ -153,10 +150,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -195,6 +192,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -203,14 +237,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -220,7 +246,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -228,7 +254,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -250,7 +291,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -265,72 +322,12 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -401,6 +398,108 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -419,18 +518,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -444,96 +531,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -603,26 +600,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -644,11 +641,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -663,25 +658,27 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -693,10 +690,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -708,130 +705,130 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1192,8 +1189,8 @@
   <sheetPr/>
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1857,10 +1854,10 @@
       <c r="C32" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E32" s="12"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -1874,7 +1871,7 @@
     <row r="33" ht="24.95" customHeight="1" spans="1:14">
       <c r="A33" s="3"/>
       <c r="B33" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>8</v>
@@ -1894,13 +1891,13 @@
     <row r="34" ht="42" customHeight="1" spans="1:14">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="4"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Revert "Revert "fw"""""
This reverts commit 07735b17f369465038d96686ed40bf44c1c63fb3.
</commit_message>
<xml_diff>
--- a/作业完成情况汇总.xlsx
+++ b/作业完成情况汇总.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24180" windowHeight="13065"/>
+    <workbookView windowWidth="28695" windowHeight="13065"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44">
   <si>
     <t>WHJ171103班晚自习作业完成情况汇总表</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>冯文</t>
+  </si>
+  <si>
+    <t>修改有问题</t>
   </si>
   <si>
     <t>沈世伟</t>
@@ -150,10 +153,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -192,6 +195,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -200,6 +211,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
@@ -215,6 +234,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -222,24 +256,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -260,14 +318,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -275,59 +325,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -398,6 +401,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -440,18 +491,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -495,42 +534,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -600,26 +603,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -641,9 +644,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -658,27 +663,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -690,10 +693,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -705,130 +708,130 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1189,8 +1192,8 @@
   <sheetPr/>
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1854,10 +1857,10 @@
       <c r="C32" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="12" t="s">
-        <v>8</v>
-      </c>
+      <c r="D32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="12"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -1871,7 +1874,7 @@
     <row r="33" ht="24.95" customHeight="1" spans="1:14">
       <c r="A33" s="3"/>
       <c r="B33" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>8</v>
@@ -1891,13 +1894,13 @@
     <row r="34" ht="42" customHeight="1" spans="1:14">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="4"/>

</xml_diff>

<commit_message>
Mzerzge branch 'master' into ccc
</commit_message>
<xml_diff>
--- a/作业完成情况汇总.xlsx
+++ b/作业完成情况汇总.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13065"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -213,10 +213,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -257,21 +257,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -283,6 +268,44 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -309,45 +332,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -369,17 +356,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -391,6 +376,21 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -419,19 +419,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -443,54 +467,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -509,13 +533,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -528,78 +600,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -705,16 +705,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -740,16 +740,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -770,10 +770,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -782,133 +782,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1029,6 +1029,11 @@
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1284,17 +1289,16 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2177,8 +2181,12 @@
       <c r="P23" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
+      <c r="Q23" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="R23" s="18" t="s">
+        <v>10</v>
+      </c>
       <c r="S23" s="18"/>
     </row>
     <row r="24" ht="24.95" customHeight="1" spans="1:19">
@@ -2530,8 +2538,12 @@
       </c>
       <c r="O32" s="18"/>
       <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
+      <c r="Q32" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="R32" s="18" t="s">
+        <v>10</v>
+      </c>
       <c r="S32" s="18"/>
     </row>
     <row r="33" ht="24.95" customHeight="1" spans="1:19">

</xml_diff>